<commit_message>
More VBA Test Codes, Added Wix Tips and Samples
</commit_message>
<xml_diff>
--- a/Excel/오늘기준_지난달_Mxx형식표현.xlsx
+++ b/Excel/오늘기준_지난달_Mxx형식표현.xlsx
@@ -1,23 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr codeName="현재_통합_문서"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitRepositories\CodeSnippet\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290FD3B1-5472-446C-9D4C-06AAA720A68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15555" windowHeight="5505"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -45,7 +55,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -383,11 +393,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="B2:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -403,7 +414,7 @@
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
         <f ca="1">TODAY()</f>
-        <v>43474</v>
+        <v>44861</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
@@ -422,49 +433,49 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C4" s="1">
-        <v>43120</v>
+        <v>44428</v>
       </c>
       <c r="D4">
-        <f ca="1">(YEAR($B$2)-YEAR(C4))*12</f>
+        <f t="shared" ref="D4:D9" ca="1" si="0">(YEAR($B$2)-YEAR(C4))*12</f>
         <v>12</v>
       </c>
       <c r="E4">
-        <f ca="1">MONTH($B$2)-MONTH(C4)</f>
-        <v>0</v>
+        <f t="shared" ref="E4:E9" ca="1" si="1">MONTH($B$2)-MONTH(C4)</f>
+        <v>2</v>
       </c>
       <c r="F4" s="2" t="str">
-        <f ca="1">CONCATENATE("M",D4+E4)</f>
-        <v>M12</v>
+        <f t="shared" ref="F4:F9" ca="1" si="2">CONCATENATE("M",D4+E4)</f>
+        <v>M14</v>
       </c>
       <c r="G4" s="2" t="str">
-        <f ca="1">CONCATENATE("M",REPT(0,2-LEN(D4+E4))&amp;(D4+E4))</f>
-        <v>M12</v>
+        <f t="shared" ref="G4:G9" ca="1" si="3">CONCATENATE("M",REPT(0,2-LEN(D4+E4))&amp;(D4+E4))</f>
+        <v>M14</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C5" s="1">
-        <v>43152</v>
+        <v>44459</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D15" ca="1" si="0">(YEAR($B$2)-YEAR(C5))*12</f>
+        <f t="shared" ca="1" si="0"/>
         <v>12</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E15" ca="1" si="1">MONTH($B$2)-MONTH(C5)</f>
-        <v>-1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
       <c r="F5" s="2" t="str">
-        <f t="shared" ref="F5:F15" ca="1" si="2">CONCATENATE("M",D5+E5)</f>
-        <v>M11</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>M13</v>
       </c>
       <c r="G5" s="2" t="str">
-        <f t="shared" ref="G5:G15" ca="1" si="3">CONCATENATE("M",REPT(0,2-LEN(D5+E5))&amp;(D5+E5))</f>
-        <v>M11</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>M13</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C6" s="1">
-        <v>43179</v>
+        <v>44489</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
@@ -472,41 +483,41 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="F6" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>M10</v>
+        <v>M12</v>
       </c>
       <c r="G6" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M10</v>
+        <v>M12</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C7" s="1">
-        <v>43210</v>
+        <v>44498</v>
       </c>
       <c r="D7">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="D7" ca="1" si="4">(YEAR($B$2)-YEAR(C7))*12</f>
         <v>12</v>
       </c>
       <c r="E7">
-        <f t="shared" ca="1" si="1"/>
-        <v>-3</v>
+        <f t="shared" ref="E7" ca="1" si="5">MONTH($B$2)-MONTH(C7)</f>
+        <v>0</v>
       </c>
       <c r="F7" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>M9</v>
+        <f t="shared" ref="F7" ca="1" si="6">CONCATENATE("M",D7+E7)</f>
+        <v>M12</v>
       </c>
       <c r="G7" s="2" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>M09</v>
+        <f t="shared" ref="G7" ca="1" si="7">CONCATENATE("M",REPT(0,2-LEN(D7+E7))&amp;(D7+E7))</f>
+        <v>M12</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C8" s="1">
-        <v>43240</v>
+        <v>44520</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
@@ -514,20 +525,20 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="F8" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>M8</v>
+        <v>M11</v>
       </c>
       <c r="G8" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M08</v>
+        <v>M11</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C9" s="1">
-        <v>43271</v>
+        <v>44561</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
@@ -535,141 +546,393 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="F9" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>M7</v>
+        <v>M10</v>
       </c>
       <c r="G9" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M07</v>
+        <v>M10</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C10" s="1">
-        <v>43301</v>
+        <v>44581</v>
       </c>
       <c r="D10">
-        <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <f ca="1">(YEAR($B$2)-YEAR(C10))*12</f>
+        <v>0</v>
       </c>
       <c r="E10">
-        <f t="shared" ca="1" si="1"/>
-        <v>-6</v>
+        <f ca="1">MONTH($B$2)-MONTH(C10)</f>
+        <v>9</v>
       </c>
       <c r="F10" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>M6</v>
+        <f ca="1">CONCATENATE("M",D10+E10)</f>
+        <v>M9</v>
       </c>
       <c r="G10" s="2" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>M06</v>
+        <f ca="1">CONCATENATE("M",REPT(0,2-LEN(D10+E10))&amp;(D10+E10))</f>
+        <v>M09</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C11" s="1">
-        <v>43332</v>
+        <v>44613</v>
       </c>
       <c r="D11">
-        <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <f t="shared" ref="D11:D21" ca="1" si="8">(YEAR($B$2)-YEAR(C11))*12</f>
+        <v>0</v>
       </c>
       <c r="E11">
-        <f t="shared" ca="1" si="1"/>
-        <v>-7</v>
+        <f t="shared" ref="E11:E21" ca="1" si="9">MONTH($B$2)-MONTH(C11)</f>
+        <v>8</v>
       </c>
       <c r="F11" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>M5</v>
+        <f t="shared" ref="F11:F21" ca="1" si="10">CONCATENATE("M",D11+E11)</f>
+        <v>M8</v>
       </c>
       <c r="G11" s="2" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>M05</v>
+        <f t="shared" ref="G11:G21" ca="1" si="11">CONCATENATE("M",REPT(0,2-LEN(D11+E11))&amp;(D11+E11))</f>
+        <v>M08</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C12" s="1">
-        <v>43363</v>
+        <v>44824</v>
       </c>
       <c r="D12">
-        <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0</v>
       </c>
       <c r="E12">
-        <f t="shared" ca="1" si="1"/>
-        <v>-8</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>1</v>
       </c>
       <c r="F12" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>M4</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>M1</v>
       </c>
       <c r="G12" s="2" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>M04</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>M01</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C13" s="1">
-        <v>43393</v>
+        <v>44854</v>
       </c>
       <c r="D13">
-        <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0</v>
       </c>
       <c r="E13">
-        <f t="shared" ca="1" si="1"/>
-        <v>-9</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>0</v>
       </c>
       <c r="F13" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>M3</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>M0</v>
       </c>
       <c r="G13" s="2" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>M03</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>M00</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C14" s="1">
-        <v>43424</v>
+        <v>44885</v>
       </c>
       <c r="D14">
-        <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0</v>
       </c>
       <c r="E14">
-        <f t="shared" ca="1" si="1"/>
-        <v>-10</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>-1</v>
       </c>
       <c r="F14" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>M2</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>M-1</v>
       </c>
       <c r="G14" s="2" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>M02</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>M-1</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C15" s="1">
-        <v>43465</v>
+        <v>44926</v>
       </c>
       <c r="D15">
-        <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0</v>
       </c>
       <c r="E15">
-        <f t="shared" ca="1" si="1"/>
-        <v>-11</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>-2</v>
       </c>
       <c r="F15" s="2" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>M1</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>M-2</v>
       </c>
       <c r="G15" s="2" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>M01</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>M-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C16" s="1">
+        <v>44946</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ca="1" si="8"/>
+        <v>-12</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ca="1" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="F16" s="2" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>M-3</v>
+      </c>
+      <c r="G16" s="2" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>M-3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C17" s="1">
+        <v>44978</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ca="1" si="8"/>
+        <v>-12</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ca="1" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="F17" s="2" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>M-4</v>
+      </c>
+      <c r="G17" s="2" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>M-4</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C18" s="1">
+        <v>45005</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ca="1" si="8"/>
+        <v>-12</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ca="1" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="F18" s="2" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>M-5</v>
+      </c>
+      <c r="G18" s="2" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>M-5</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C19" s="1">
+        <v>45036</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ca="1" si="8"/>
+        <v>-12</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ca="1" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="F19" s="2" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>M-6</v>
+      </c>
+      <c r="G19" s="2" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>M-6</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C20" s="1">
+        <v>45066</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ca="1" si="8"/>
+        <v>-12</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ca="1" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="F20" s="2" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>M-7</v>
+      </c>
+      <c r="G20" s="2" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>M-7</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C21" s="1">
+        <v>45097</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ca="1" si="8"/>
+        <v>-12</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ca="1" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="F21" s="2" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>M-8</v>
+      </c>
+      <c r="G21" s="2" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>M-8</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C22" s="1">
+        <v>45127</v>
+      </c>
+      <c r="D22">
+        <f ca="1">(YEAR($B$2)-YEAR(C22))*12</f>
+        <v>-12</v>
+      </c>
+      <c r="E22">
+        <f ca="1">MONTH($B$2)-MONTH(C22)</f>
+        <v>3</v>
+      </c>
+      <c r="F22" s="2" t="str">
+        <f ca="1">CONCATENATE("M",D22+E22)</f>
+        <v>M-9</v>
+      </c>
+      <c r="G22" s="2" t="str">
+        <f ca="1">CONCATENATE("M",REPT(0,2-LEN(D22+E22))&amp;(D22+E22))</f>
+        <v>M-9</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C23" s="1">
+        <v>45158</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ref="D23:D27" ca="1" si="12">(YEAR($B$2)-YEAR(C23))*12</f>
+        <v>-12</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ref="E23:E27" ca="1" si="13">MONTH($B$2)-MONTH(C23)</f>
+        <v>2</v>
+      </c>
+      <c r="F23" s="2" t="str">
+        <f t="shared" ref="F23:F27" ca="1" si="14">CONCATENATE("M",D23+E23)</f>
+        <v>M-10</v>
+      </c>
+      <c r="G23" s="2" t="e">
+        <f t="shared" ref="G23:G27" ca="1" si="15">CONCATENATE("M",REPT(0,2-LEN(D23+E23))&amp;(D23+E23))</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C24" s="1">
+        <v>45189</v>
+      </c>
+      <c r="D24">
+        <f t="shared" ref="D24" ca="1" si="16">(YEAR($B$2)-YEAR(C24))*12</f>
+        <v>-12</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ref="E24" ca="1" si="17">MONTH($B$2)-MONTH(C24)</f>
+        <v>1</v>
+      </c>
+      <c r="F24" s="2" t="str">
+        <f t="shared" ref="F24" ca="1" si="18">CONCATENATE("M",D24+E24)</f>
+        <v>M-11</v>
+      </c>
+      <c r="G24" s="2" t="e">
+        <f t="shared" ref="G24" ca="1" si="19">CONCATENATE("M",REPT(0,2-LEN(D24+E24))&amp;(D24+E24))</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C25" s="1">
+        <v>45219</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ca="1" si="12"/>
+        <v>-12</v>
+      </c>
+      <c r="E25">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="2" t="str">
+        <f t="shared" ca="1" si="14"/>
+        <v>M-12</v>
+      </c>
+      <c r="G25" s="2" t="e">
+        <f t="shared" ca="1" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C26" s="1">
+        <v>45250</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ca="1" si="12"/>
+        <v>-12</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ca="1" si="13"/>
+        <v>-1</v>
+      </c>
+      <c r="F26" s="2" t="str">
+        <f t="shared" ca="1" si="14"/>
+        <v>M-13</v>
+      </c>
+      <c r="G26" s="2" t="e">
+        <f t="shared" ca="1" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C27" s="1">
+        <v>45291</v>
+      </c>
+      <c r="D27">
+        <f t="shared" ca="1" si="12"/>
+        <v>-12</v>
+      </c>
+      <c r="E27">
+        <f t="shared" ca="1" si="13"/>
+        <v>-2</v>
+      </c>
+      <c r="F27" s="2" t="str">
+        <f t="shared" ca="1" si="14"/>
+        <v>M-14</v>
+      </c>
+      <c r="G27" s="2" t="e">
+        <f t="shared" ca="1" si="15"/>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated codes for Excel VBA, WEBAPI Samples
</commit_message>
<xml_diff>
--- a/Excel/오늘기준_지난달_Mxx형식표현.xlsx
+++ b/Excel/오늘기준_지난달_Mxx형식표현.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr codeName="현재_통합_문서"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitRepositories\CodeSnippet\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290FD3B1-5472-446C-9D4C-06AAA720A68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C41C8D-0CED-4C92-B91B-5340F0347DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -398,7 +398,7 @@
   <dimension ref="B2:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -414,7 +414,7 @@
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
         <f ca="1">TODAY()</f>
-        <v>44861</v>
+        <v>44959</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
@@ -437,19 +437,19 @@
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D9" ca="1" si="0">(YEAR($B$2)-YEAR(C4))*12</f>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E9" ca="1" si="1">MONTH($B$2)-MONTH(C4)</f>
-        <v>2</v>
+        <v>-6</v>
       </c>
       <c r="F4" s="2" t="str">
         <f t="shared" ref="F4:F9" ca="1" si="2">CONCATENATE("M",D4+E4)</f>
-        <v>M14</v>
+        <v>M18</v>
       </c>
       <c r="G4" s="2" t="str">
         <f t="shared" ref="G4:G9" ca="1" si="3">CONCATENATE("M",REPT(0,2-LEN(D4+E4))&amp;(D4+E4))</f>
-        <v>M14</v>
+        <v>M18</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
@@ -458,19 +458,19 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>-7</v>
       </c>
       <c r="F5" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>M13</v>
+        <v>M17</v>
       </c>
       <c r="G5" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M13</v>
+        <v>M17</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
@@ -479,19 +479,19 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="F6" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>M12</v>
+        <v>M16</v>
       </c>
       <c r="G6" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M12</v>
+        <v>M16</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
@@ -500,19 +500,19 @@
       </c>
       <c r="D7">
         <f t="shared" ref="D7" ca="1" si="4">(YEAR($B$2)-YEAR(C7))*12</f>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E7">
         <f t="shared" ref="E7" ca="1" si="5">MONTH($B$2)-MONTH(C7)</f>
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="F7" s="2" t="str">
         <f t="shared" ref="F7" ca="1" si="6">CONCATENATE("M",D7+E7)</f>
-        <v>M12</v>
+        <v>M16</v>
       </c>
       <c r="G7" s="2" t="str">
         <f t="shared" ref="G7" ca="1" si="7">CONCATENATE("M",REPT(0,2-LEN(D7+E7))&amp;(D7+E7))</f>
-        <v>M12</v>
+        <v>M16</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
@@ -521,19 +521,19 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>-1</v>
+        <v>-9</v>
       </c>
       <c r="F8" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>M11</v>
+        <v>M15</v>
       </c>
       <c r="G8" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M11</v>
+        <v>M15</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
@@ -542,19 +542,19 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>-2</v>
+        <v>-10</v>
       </c>
       <c r="F9" s="2" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>M10</v>
+        <v>M14</v>
       </c>
       <c r="G9" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M10</v>
+        <v>M14</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
@@ -563,19 +563,19 @@
       </c>
       <c r="D10">
         <f ca="1">(YEAR($B$2)-YEAR(C10))*12</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E10">
         <f ca="1">MONTH($B$2)-MONTH(C10)</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F10" s="2" t="str">
         <f ca="1">CONCATENATE("M",D10+E10)</f>
-        <v>M9</v>
+        <v>M13</v>
       </c>
       <c r="G10" s="2" t="str">
         <f ca="1">CONCATENATE("M",REPT(0,2-LEN(D10+E10))&amp;(D10+E10))</f>
-        <v>M09</v>
+        <v>M13</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
@@ -584,19 +584,19 @@
       </c>
       <c r="D11">
         <f t="shared" ref="D11:D21" ca="1" si="8">(YEAR($B$2)-YEAR(C11))*12</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:E21" ca="1" si="9">MONTH($B$2)-MONTH(C11)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F11" s="2" t="str">
         <f t="shared" ref="F11:F21" ca="1" si="10">CONCATENATE("M",D11+E11)</f>
-        <v>M8</v>
+        <v>M12</v>
       </c>
       <c r="G11" s="2" t="str">
         <f t="shared" ref="G11:G21" ca="1" si="11">CONCATENATE("M",REPT(0,2-LEN(D11+E11))&amp;(D11+E11))</f>
-        <v>M08</v>
+        <v>M12</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
@@ -605,19 +605,19 @@
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>-7</v>
       </c>
       <c r="F12" s="2" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>M1</v>
+        <v>M5</v>
       </c>
       <c r="G12" s="2" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>M01</v>
+        <v>M05</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
@@ -626,19 +626,19 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="9"/>
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="F13" s="2" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>M0</v>
+        <v>M4</v>
       </c>
       <c r="G13" s="2" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>M00</v>
+        <v>M04</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
@@ -647,19 +647,19 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="9"/>
-        <v>-1</v>
+        <v>-9</v>
       </c>
       <c r="F14" s="2" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>M-1</v>
+        <v>M3</v>
       </c>
       <c r="G14" s="2" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>M-1</v>
+        <v>M03</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
@@ -668,19 +668,19 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="9"/>
-        <v>-2</v>
+        <v>-10</v>
       </c>
       <c r="F15" s="2" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>M-2</v>
+        <v>M2</v>
       </c>
       <c r="G15" s="2" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>M-2</v>
+        <v>M02</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
@@ -689,19 +689,19 @@
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="8"/>
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="9"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F16" s="2" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>M-3</v>
+        <v>M1</v>
       </c>
       <c r="G16" s="2" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>M-3</v>
+        <v>M01</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.3">
@@ -710,19 +710,19 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="8"/>
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="9"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F17" s="2" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>M-4</v>
+        <v>M0</v>
       </c>
       <c r="G17" s="2" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>M-4</v>
+        <v>M00</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.3">
@@ -731,19 +731,19 @@
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="8"/>
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="9"/>
-        <v>7</v>
+        <v>-1</v>
       </c>
       <c r="F18" s="2" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>M-5</v>
+        <v>M-1</v>
       </c>
       <c r="G18" s="2" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>M-5</v>
+        <v>M-1</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.3">
@@ -752,19 +752,19 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="8"/>
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="9"/>
-        <v>6</v>
+        <v>-2</v>
       </c>
       <c r="F19" s="2" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>M-6</v>
+        <v>M-2</v>
       </c>
       <c r="G19" s="2" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>M-6</v>
+        <v>M-2</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.3">
@@ -773,19 +773,19 @@
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="8"/>
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="9"/>
-        <v>5</v>
+        <v>-3</v>
       </c>
       <c r="F20" s="2" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>M-7</v>
+        <v>M-3</v>
       </c>
       <c r="G20" s="2" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>M-7</v>
+        <v>M-3</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.3">
@@ -794,19 +794,19 @@
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="8"/>
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="9"/>
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="F21" s="2" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>M-8</v>
+        <v>M-4</v>
       </c>
       <c r="G21" s="2" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>M-8</v>
+        <v>M-4</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.3">
@@ -815,19 +815,19 @@
       </c>
       <c r="D22">
         <f ca="1">(YEAR($B$2)-YEAR(C22))*12</f>
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <f ca="1">MONTH($B$2)-MONTH(C22)</f>
-        <v>3</v>
+        <v>-5</v>
       </c>
       <c r="F22" s="2" t="str">
         <f ca="1">CONCATENATE("M",D22+E22)</f>
-        <v>M-9</v>
+        <v>M-5</v>
       </c>
       <c r="G22" s="2" t="str">
         <f ca="1">CONCATENATE("M",REPT(0,2-LEN(D22+E22))&amp;(D22+E22))</f>
-        <v>M-9</v>
+        <v>M-5</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.3">
@@ -836,19 +836,19 @@
       </c>
       <c r="D23">
         <f t="shared" ref="D23:D27" ca="1" si="12">(YEAR($B$2)-YEAR(C23))*12</f>
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <f t="shared" ref="E23:E27" ca="1" si="13">MONTH($B$2)-MONTH(C23)</f>
-        <v>2</v>
+        <v>-6</v>
       </c>
       <c r="F23" s="2" t="str">
         <f t="shared" ref="F23:F27" ca="1" si="14">CONCATENATE("M",D23+E23)</f>
-        <v>M-10</v>
-      </c>
-      <c r="G23" s="2" t="e">
+        <v>M-6</v>
+      </c>
+      <c r="G23" s="2" t="str">
         <f t="shared" ref="G23:G27" ca="1" si="15">CONCATENATE("M",REPT(0,2-LEN(D23+E23))&amp;(D23+E23))</f>
-        <v>#VALUE!</v>
+        <v>M-6</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.3">
@@ -857,19 +857,19 @@
       </c>
       <c r="D24">
         <f t="shared" ref="D24" ca="1" si="16">(YEAR($B$2)-YEAR(C24))*12</f>
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <f t="shared" ref="E24" ca="1" si="17">MONTH($B$2)-MONTH(C24)</f>
-        <v>1</v>
+        <v>-7</v>
       </c>
       <c r="F24" s="2" t="str">
         <f t="shared" ref="F24" ca="1" si="18">CONCATENATE("M",D24+E24)</f>
-        <v>M-11</v>
-      </c>
-      <c r="G24" s="2" t="e">
+        <v>M-7</v>
+      </c>
+      <c r="G24" s="2" t="str">
         <f t="shared" ref="G24" ca="1" si="19">CONCATENATE("M",REPT(0,2-LEN(D24+E24))&amp;(D24+E24))</f>
-        <v>#VALUE!</v>
+        <v>M-7</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.3">
@@ -878,19 +878,19 @@
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="12"/>
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="F25" s="2" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>M-12</v>
-      </c>
-      <c r="G25" s="2" t="e">
+        <v>M-8</v>
+      </c>
+      <c r="G25" s="2" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>#VALUE!</v>
+        <v>M-8</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.3">
@@ -899,19 +899,19 @@
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="12"/>
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="13"/>
-        <v>-1</v>
+        <v>-9</v>
       </c>
       <c r="F26" s="2" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>M-13</v>
-      </c>
-      <c r="G26" s="2" t="e">
+        <v>M-9</v>
+      </c>
+      <c r="G26" s="2" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>#VALUE!</v>
+        <v>M-9</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.3">
@@ -920,15 +920,15 @@
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="12"/>
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="13"/>
-        <v>-2</v>
+        <v>-10</v>
       </c>
       <c r="F27" s="2" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>M-14</v>
+        <v>M-10</v>
       </c>
       <c r="G27" s="2" t="e">
         <f t="shared" ca="1" si="15"/>

</xml_diff>